<commit_message>
test implementacion de js
</commit_message>
<xml_diff>
--- a/public/u_excel/1.DP.1.xlsx
+++ b/public/u_excel/1.DP.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zizek\Desktop\Repositorio\dev-bomberos\public\u_excel\geografico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zizek\Desktop\Repositorio\dev-bomberos\public\u_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2369F1AE-8240-47EB-99BC-476939EA6011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D341EF-58C5-42F8-A8C6-C9A530475B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t xml:space="preserve">Localidad, Municipio </t>
   </si>
@@ -39,54 +39,12 @@
   <si>
     <t>Superficie                                                              (Ha)</t>
   </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nota:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> La superficie de la ciudad corresponde a las áreas urbanas y la del municipio a la continental.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Fuente:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Elaboración propia IMIP con datos del INEGI.</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,13 +201,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="5" tint="-0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="5" tint="-0.499984740745262"/>
       <name val="Arial"/>
@@ -662,12 +613,12 @@
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1015,22 +966,24 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="24.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="24.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="12">
+      <c r="A1" s="11">
         <v>2010</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1075,12 +1028,12 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>2020</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1126,22 +1079,18 @@
         <v>4.24709503136636</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C15" s="10"/>

</xml_diff>